<commit_message>
ploting results about number of filters
</commit_message>
<xml_diff>
--- a/error/new/fabric_layer_impact/fabric.xlsx
+++ b/error/new/fabric_layer_impact/fabric.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
   <si>
     <t>epochs</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>4 layers</t>
+  </si>
+  <si>
+    <t>threshold</t>
   </si>
 </sst>
 </file>
@@ -228,10 +231,17 @@
           </c:dPt>
           <c:cat>
             <c:numRef>
-              <c:f>Folha1!$A$3:$A$23</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$A$3:$A$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$A$3:$A$7,Folha1!$A$9:$A$23)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -248,51 +258,48 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>45</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>50</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>55</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>60</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>65</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>70</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>75</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>80</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>85</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>90</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="20">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -300,10 +307,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Folha1!$B$3:$B$8</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$B$3:$B$8</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Folha1!$B$3:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -317,9 +331,6 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -352,10 +363,17 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Folha1!$A$3:$A$23</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$A$3:$A$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$A$3:$A$7,Folha1!$A$9:$A$23)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -372,51 +390,48 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>45</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>50</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>55</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>60</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>65</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>70</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>75</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>80</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>85</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>90</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="20">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -424,10 +439,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Folha1!$C$3:$C$8</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$C$3:$C$8</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Folha1!$C$3:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -441,9 +463,6 @@
                   <c:v>99.61</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>99.61</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>99.61</c:v>
                 </c:pt>
               </c:numCache>
@@ -473,10 +492,17 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Folha1!$A$3:$A$23</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$A$3:$A$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$A$3:$A$7,Folha1!$A$9:$A$23)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -493,51 +519,48 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>45</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>50</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>55</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>60</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>65</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>70</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>75</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>80</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>85</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>90</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="20">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -545,10 +568,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Folha1!$D$3:$D$8</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$D$3:$D$8</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Folha1!$D$3:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -562,9 +592,6 @@
                   <c:v>96.43</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>99.11</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>99.11</c:v>
                 </c:pt>
               </c:numCache>
@@ -597,10 +624,17 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Folha1!$A$3:$A$23</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$A$3:$A$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$A$3:$A$7,Folha1!$A$9:$A$23)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -669,6 +703,13 @@
           </c:cat>
           <c:val>
             <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$G$3:$G$7</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>Folha1!$G$3:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -683,9 +724,6 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="4">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -718,10 +756,17 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Folha1!$A$3:$A$23</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$A$3:$A$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$A$3:$A$7,Folha1!$A$9:$A$23)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -790,6 +835,13 @@
           </c:cat>
           <c:val>
             <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$H$3:$H$7</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>Folha1!$H$3:$H$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -804,9 +856,6 @@
                   <c:v>99.61</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="4">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -836,10 +885,17 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Folha1!$A$3:$A$23</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$A$3:$A$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$A$3:$A$7,Folha1!$A$9:$A$23)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -908,6 +964,13 @@
           </c:cat>
           <c:val>
             <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$I$3:$I$7</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>Folha1!$I$3:$I$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -922,9 +985,6 @@
                   <c:v>97.32</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>99.11</c:v>
-                </c:pt>
-                <c:pt idx="4">
                   <c:v>99.11</c:v>
                 </c:pt>
               </c:numCache>
@@ -957,10 +1017,17 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Folha1!$A$3:$A$23</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$A$3:$A$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$A$3:$A$7,Folha1!$A$9:$A$23)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1029,6 +1096,13 @@
           </c:cat>
           <c:val>
             <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$L$3:$L$6</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>Folha1!$L$3:$L$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -1040,9 +1114,6 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -1075,10 +1146,17 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Folha1!$A$3:$A$23</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$A$3:$A$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$A$3:$A$7,Folha1!$A$9:$A$23)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1147,6 +1225,13 @@
           </c:cat>
           <c:val>
             <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$M$3:$M$6</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>Folha1!$M$3:$M$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -1158,9 +1243,6 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -1247,10 +1329,17 @@
           </c:dPt>
           <c:cat>
             <c:numRef>
-              <c:f>Folha1!$A$3:$A$23</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$A$3:$A$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$A$3:$A$7,Folha1!$A$9:$A$23)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1319,6 +1408,13 @@
           </c:cat>
           <c:val>
             <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$N$3:$N$6</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>Folha1!$N$3:$N$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -1330,9 +1426,6 @@
                   <c:v>97.32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -1365,10 +1458,17 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Folha1!$A$3:$A$23</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$A$3:$A$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$A$3:$A$7,Folha1!$A$9:$A$23)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1437,6 +1537,13 @@
           </c:cat>
           <c:val>
             <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$Q$3:$Q$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>Folha1!$Q$3:$Q$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -1445,9 +1552,6 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="2">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -1480,10 +1584,17 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Folha1!$A$3:$A$23</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$A$3:$A$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$A$3:$A$7,Folha1!$A$9:$A$23)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1552,6 +1663,13 @@
           </c:cat>
           <c:val>
             <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$R$3:$R$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>Folha1!$R$3:$R$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -1560,9 +1678,6 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="2">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -1592,10 +1707,17 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Folha1!$A$3:$A$23</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$A$3:$A$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$A$3:$A$7,Folha1!$A$9:$A$23)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1664,6 +1786,13 @@
           </c:cat>
           <c:val>
             <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$S$3:$S$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>Folha1!$S$3:$S$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -1672,9 +1801,6 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="2">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -1734,10 +1860,17 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Folha1!$A$3:$A$23</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$A$3:$A$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$A$3:$A$7,Folha1!$A$9:$A$23)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1754,51 +1887,48 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>45</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>50</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>55</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>60</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>65</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>70</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>75</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>80</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>85</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>90</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="20">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -1806,10 +1936,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Folha1!$E$3:$E$8</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$E$3:$E$8</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Folha1!$E$3:$E$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1823,9 +1960,6 @@
                   <c:v>81.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>93.75</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>93.75</c:v>
                 </c:pt>
               </c:numCache>
@@ -1870,10 +2004,17 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Folha1!$A$3:$A$23</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$A$3:$A$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$A$3:$A$7,Folha1!$A$9:$A$23)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1942,6 +2083,13 @@
           </c:cat>
           <c:val>
             <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$J$3:$J$7</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>Folha1!$J$3:$J$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -1956,9 +2104,6 @@
                   <c:v>81.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>93.75</c:v>
-                </c:pt>
-                <c:pt idx="4">
                   <c:v>93.75</c:v>
                 </c:pt>
               </c:numCache>
@@ -2003,10 +2148,17 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Folha1!$A$3:$A$23</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$A$3:$A$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$A$3:$A$7,Folha1!$A$9:$A$23)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2075,6 +2227,13 @@
           </c:cat>
           <c:val>
             <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$O$3:$O$6</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>Folha1!$O$3:$O$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -2086,9 +2245,6 @@
                   <c:v>81.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -2133,10 +2289,17 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Folha1!$A$3:$A$23</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$A$3:$A$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$A$3:$A$7,Folha1!$A$9:$A$23)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2205,6 +2368,13 @@
           </c:cat>
           <c:val>
             <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$T$3:$T$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>Folha1!$T$3:$T$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -2213,9 +2383,6 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="2">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -2225,6 +2392,91 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000012-667E-446C-99DA-F8752E640BA3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="16"/>
+          <c:order val="16"/>
+          <c:tx>
+            <c:v>stop_criteria</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="3175" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="lgDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="5"/>
+              <c:pt idx="0">
+                <c:v>0</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>5</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>10</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>15</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>20</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>25</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$V$3:$V$7</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Folha1!$V$3:$V$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>97.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-A864-438C-844D-7D00C9E27004}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3439,15 +3691,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T23"/>
+  <dimension ref="A1:V23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="W11" sqref="W11"/>
+      <selection activeCell="W28" sqref="W28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="3" t="s">
         <v>5</v>
@@ -3477,7 +3729,7 @@
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3532,8 +3784,11 @@
       <c r="T2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="V2" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -3585,8 +3840,11 @@
       <c r="T3">
         <v>0</v>
       </c>
+      <c r="V3">
+        <v>97.5</v>
+      </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>5</v>
       </c>
@@ -3638,8 +3896,11 @@
       <c r="T4">
         <v>100</v>
       </c>
+      <c r="V4">
+        <v>97.5</v>
+      </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>10</v>
       </c>
@@ -3679,20 +3940,11 @@
       <c r="O5">
         <v>100</v>
       </c>
-      <c r="Q5">
-        <v>100</v>
-      </c>
-      <c r="R5">
-        <v>100</v>
-      </c>
-      <c r="S5">
-        <v>100</v>
-      </c>
-      <c r="T5">
-        <v>100</v>
+      <c r="V5">
+        <v>97.5</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>15</v>
       </c>
@@ -3720,20 +3972,11 @@
       <c r="J6">
         <v>93.75</v>
       </c>
-      <c r="L6">
-        <v>100</v>
-      </c>
-      <c r="M6">
-        <v>100</v>
-      </c>
-      <c r="N6">
-        <v>100</v>
-      </c>
-      <c r="O6">
-        <v>100</v>
+      <c r="V6">
+        <v>97.5</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>20</v>
       </c>
@@ -3749,109 +3992,136 @@
       <c r="E7">
         <v>93.75</v>
       </c>
-      <c r="G7">
-        <v>100</v>
-      </c>
-      <c r="H7">
-        <v>100</v>
-      </c>
-      <c r="I7">
-        <v>99.11</v>
-      </c>
-      <c r="J7">
-        <v>93.75</v>
+      <c r="V7">
+        <v>97.5</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>25</v>
       </c>
-      <c r="B8">
-        <v>100</v>
-      </c>
-      <c r="C8">
-        <v>99.61</v>
-      </c>
-      <c r="D8">
-        <v>99.11</v>
-      </c>
-      <c r="E8">
-        <v>93.75</v>
+      <c r="V8">
+        <v>97.5</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>30</v>
       </c>
+      <c r="V9">
+        <v>97.5</v>
+      </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>35</v>
       </c>
+      <c r="V10">
+        <v>97.5</v>
+      </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>40</v>
       </c>
+      <c r="V11">
+        <v>97.5</v>
+      </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>45</v>
       </c>
+      <c r="V12">
+        <v>97.5</v>
+      </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>50</v>
       </c>
+      <c r="V13">
+        <v>97.5</v>
+      </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>55</v>
       </c>
+      <c r="V14">
+        <v>97.5</v>
+      </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>60</v>
       </c>
+      <c r="V15">
+        <v>97.5</v>
+      </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>65</v>
       </c>
+      <c r="V16">
+        <v>97.5</v>
+      </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>70</v>
       </c>
+      <c r="V17">
+        <v>97.5</v>
+      </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>75</v>
       </c>
+      <c r="V18">
+        <v>97.5</v>
+      </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>80</v>
       </c>
+      <c r="V19">
+        <v>97.5</v>
+      </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>85</v>
       </c>
+      <c r="V20">
+        <v>97.5</v>
+      </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>90</v>
       </c>
+      <c r="V21">
+        <v>97.5</v>
+      </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>95</v>
       </c>
+      <c r="V22">
+        <v>97.5</v>
+      </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>100</v>
+      </c>
+      <c r="V23">
+        <v>97.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
maybe try testing batch size?
</commit_message>
<xml_diff>
--- a/error/new/fabric_layer_impact/fabric.xlsx
+++ b/error/new/fabric_layer_impact/fabric.xlsx
@@ -604,6 +604,137 @@
           </c:extLst>
         </c:ser>
         <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>1layer_min</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$A$3:$A$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$A$3:$A$7,Folha1!$A$9:$A$23)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$E$3:$E$8</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Folha1!$E$3:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>56.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>81.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>93.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-667E-446C-99DA-F8752E640BA3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
@@ -993,6 +1124,137 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-667E-446C-99DA-F8752E640BA3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>2layers_min</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$A$3:$A$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$A$3:$A$7,Folha1!$A$9:$A$23)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$J$3:$J$7</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Folha1!$J$3:$J$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>37.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>81.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>93.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-667E-446C-99DA-F8752E640BA3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1438,6 +1700,134 @@
           </c:extLst>
         </c:ser>
         <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:v>3layers_min</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$A$3:$A$23</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Folha1!$A$3:$A$7,Folha1!$A$9:$A$23)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$O$3:$O$6</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Folha1!$O$3:$O$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>81.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-667E-446C-99DA-F8752E640BA3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="12"/>
           <c:order val="12"/>
           <c:tx>
@@ -1812,451 +2202,6 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="500"/>
-        <c:overlap val="-75"/>
-        <c:axId val="275492384"/>
-        <c:axId val="275489432"/>
-      </c:barChart>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>1layer_min</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>Folha1!$A$3:$A$23</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>(Folha1!$A$3:$A$7,Folha1!$A$9:$A$23)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>100</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>Folha1!$E$3:$E$8</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>Folha1!$E$3:$E$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43.75</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>56.25</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>81.25</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>93.75</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-667E-446C-99DA-F8752E640BA3}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:tx>
-            <c:v>2layers_min</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>Folha1!$A$3:$A$23</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>(Folha1!$A$3:$A$7,Folha1!$A$9:$A$23)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>100</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>Folha1!$J$3:$J$7</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>Folha1!$J$3:$J$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>37.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>81.25</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>93.75</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-667E-446C-99DA-F8752E640BA3}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="11"/>
-          <c:order val="11"/>
-          <c:tx>
-            <c:v>3layers_min</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>Folha1!$A$3:$A$23</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>(Folha1!$A$3:$A$7,Folha1!$A$9:$A$23)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>100</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>Folha1!$O$3:$O$6</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>Folha1!$O$3:$O$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>81.25</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>100</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000D-667E-446C-99DA-F8752E640BA3}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
         <c:ser>
           <c:idx val="15"/>
           <c:order val="15"/>
@@ -2264,29 +2209,17 @@
             <c:v>4layers_min</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent6"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:extLst>
@@ -2388,13 +2321,27 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000012-667E-446C-99DA-F8752E640BA3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="500"/>
+        <c:axId val="275492384"/>
+        <c:axId val="275489432"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="16"/>
           <c:order val="16"/>
@@ -3391,14 +3338,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>112776</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>129540</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>3048</xdr:rowOff>
     </xdr:to>

</xml_diff>